<commit_message>
Add database query file
</commit_message>
<xml_diff>
--- a/Databases/Helperland - Database.xlsx
+++ b/Databases/Helperland - Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Tatva Soft\Helperland\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AACF68F-ED13-4440-96A6-7E549952F256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADEEE8F-6753-4A75-B427-D8CAF7BC2471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{97C08BD9-FCDA-494F-8F00-8F7E3D9A4233}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="80">
   <si>
     <t>Customer Table</t>
   </si>
@@ -111,9 +109,6 @@
     <t>varchar</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Address Table</t>
   </si>
   <si>
@@ -132,18 +127,9 @@
     <t>UserType</t>
   </si>
   <si>
-    <t>ENUM</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>(0,1,2)</t>
-  </si>
-  <si>
-    <t>(0,1)</t>
-  </si>
-  <si>
     <t>Services Table</t>
   </si>
   <si>
@@ -201,21 +187,12 @@
     <t>date</t>
   </si>
   <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
     <t>(0,1,2,3,4)</t>
   </si>
   <si>
-    <t>(1,2,3,4,5)</t>
-  </si>
-  <si>
     <t>Cancle Reason</t>
   </si>
   <si>
@@ -246,9 +223,6 @@
     <t>Constraint</t>
   </si>
   <si>
-    <t>Primary Key</t>
-  </si>
-  <si>
     <t>Not Null</t>
   </si>
   <si>
@@ -267,19 +241,37 @@
     <t xml:space="preserve"> - </t>
   </si>
   <si>
-    <t xml:space="preserve"> Unique</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
     <t>Foreign Key (Cust-id , Customer Table)</t>
   </si>
   <si>
     <t>Foreign Key (SP-id , Service Provider Table)</t>
   </si>
   <si>
-    <t>Primary Key , Foreign Key (Cust-id , Customer Table)</t>
+    <t>float</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Foreign Key (Cust-id , Customer Table)</t>
+  </si>
+  <si>
+    <t>Primary Key , Auto increment</t>
+  </si>
+  <si>
+    <t>Primary Key , Auto Increment</t>
+  </si>
+  <si>
+    <t>Check (arriaval Rating IN(1,2,3,4,5))</t>
+  </si>
+  <si>
+    <t>Check(userType IN(0,1,2))</t>
+  </si>
+  <si>
+    <t>Check (Status IN(0,1))</t>
   </si>
 </sst>
 </file>
@@ -340,7 +332,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -424,11 +416,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -457,9 +458,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -468,24 +466,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -508,6 +488,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD44B8D5-4AEC-44C8-BFF7-9D4A44C72100}">
   <dimension ref="B2:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,11 +851,9 @@
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
@@ -845,9 +861,7 @@
     <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -856,54 +870,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="4" t="s">
+      <c r="H3" s="36" t="s">
         <v>7</v>
       </c>
+      <c r="K3" s="17"/>
     </row>
     <row r="4" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -922,23 +925,12 @@
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -954,117 +946,84 @@
         <v>20</v>
       </c>
       <c r="F5" s="4">
-        <v>30</v>
-      </c>
-      <c r="G5" s="4">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="6">
-        <v>20</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="4">
-        <v>20</v>
-      </c>
+      <c r="H5" s="4">
+        <v>50</v>
+      </c>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>74</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="K6" s="30"/>
     </row>
     <row r="7" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="K7" s="30"/>
     </row>
     <row r="9" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
     </row>
     <row r="10" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -1080,44 +1039,35 @@
         <v>4</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="4" t="s">
+      <c r="H10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="I10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="J10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="K10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="L10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="M10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="N10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="R10" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
     </row>
     <row r="11" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
@@ -1133,44 +1083,35 @@
         <v>24</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R11" s="10" t="s">
-        <v>32</v>
-      </c>
+      <c r="H11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
     </row>
     <row r="12" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
@@ -1186,221 +1127,194 @@
         <v>20</v>
       </c>
       <c r="F12" s="4">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="9">
+        <v>20</v>
+      </c>
+      <c r="I12" s="10">
+        <v>15</v>
+      </c>
+      <c r="J12" s="10">
         <v>30</v>
       </c>
-      <c r="G12" s="4">
-        <v>10</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="6">
+      <c r="K12" s="10">
         <v>20</v>
       </c>
-      <c r="J12" s="4">
-        <v>15</v>
-      </c>
-      <c r="K12" s="4">
-        <v>10</v>
-      </c>
-      <c r="L12" s="4">
-        <v>25</v>
-      </c>
-      <c r="M12" s="4">
-        <v>25</v>
-      </c>
-      <c r="N12" s="4">
+      <c r="L12" s="10">
+        <v>10</v>
+      </c>
+      <c r="M12" s="10">
+        <v>6</v>
+      </c>
+      <c r="N12" s="7">
         <v>20</v>
       </c>
-      <c r="O12" s="4">
-        <v>6</v>
-      </c>
-      <c r="P12" s="4">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>35</v>
-      </c>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
     </row>
     <row r="13" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="26" t="s">
-        <v>68</v>
+      <c r="B13" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>71</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
     </row>
     <row r="14" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
-        <v>69</v>
+      <c r="B14" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>76</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
     </row>
     <row r="15" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
     </row>
     <row r="16" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="B16" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
     </row>
     <row r="17" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
     </row>
     <row r="18" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
@@ -1416,10 +1330,10 @@
         <v>10</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
@@ -1430,72 +1344,72 @@
         <v>5</v>
       </c>
       <c r="D19" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E19" s="6">
-        <v>20</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>35</v>
+        <v>255</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="26" t="s">
-        <v>68</v>
+      <c r="B20" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
-        <v>69</v>
+      <c r="B21" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B23" s="22"/>
+      <c r="B23" s="15"/>
     </row>
     <row r="24" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
+      <c r="B24" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -1506,10 +1420,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>18</v>
@@ -1544,13 +1458,13 @@
         <v>10</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
@@ -1564,177 +1478,177 @@
         <v>5</v>
       </c>
       <c r="E27" s="4">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F27" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G27" s="4">
         <v>6</v>
       </c>
       <c r="H27" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I27" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B28" s="26" t="s">
-        <v>68</v>
+      <c r="B28" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="E29" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="26"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="26"/>
+      <c r="X32" s="26"/>
+      <c r="Y32" s="27"/>
+    </row>
+    <row r="33" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="19"/>
-    </row>
-    <row r="33" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="28" t="s">
+      <c r="J33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="L33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="M33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="O33" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="P33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="Q33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N33" s="2" t="s">
+      <c r="R33" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O33" s="2" t="s">
+      <c r="S33" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P33" s="2" t="s">
+      <c r="T33" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q33" s="2" t="s">
+      <c r="U33" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R33" s="2" t="s">
+      <c r="V33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="T33" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="U33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="V33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="W33" s="2" t="s">
+      <c r="X33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="X33" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y33" s="2" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="34" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="11" t="s">
@@ -1750,52 +1664,52 @@
         <v>23</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="Q34" s="2" t="s">
         <v>10</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="U34" s="2" t="s">
         <v>10</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="W34" s="2" t="s">
         <v>23</v>
@@ -1808,7 +1722,7 @@
       </c>
     </row>
     <row r="35" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="11">
@@ -1854,216 +1768,216 @@
         <v>5</v>
       </c>
       <c r="Q35" s="2">
-        <v>50</v>
-      </c>
-      <c r="R35" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="S35" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="T35" s="2" t="s">
-        <v>59</v>
+        <v>255</v>
+      </c>
+      <c r="R35" s="2">
+        <v>1</v>
+      </c>
+      <c r="S35" s="2">
+        <v>1</v>
+      </c>
+      <c r="T35" s="2">
+        <v>1</v>
       </c>
       <c r="U35" s="2">
         <v>50</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="W35" s="2">
         <v>5</v>
       </c>
       <c r="X35" s="2">
-        <v>30</v>
+        <v>255</v>
       </c>
       <c r="Y35" s="2">
-        <v>30</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B36" s="26" t="s">
-        <v>68</v>
+      <c r="B36" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="U36" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="Y36" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="E37" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="I37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="J37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="K37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="L37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="M37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="N37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="O37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="P37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="R37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="S37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="T37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="U37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="V37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="W37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="X37" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y37" s="29" t="s">
-        <v>76</v>
+        <v>68</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="L37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="M37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="N37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="O37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="P37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="R37" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="S37" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="T37" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="U37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="V37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="W37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="X37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y37" s="22" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
+      <c r="B40" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
       <c r="E40" s="3"/>
-      <c r="G40" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
+      <c r="G40" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
     </row>
     <row r="41" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="G41" s="13" t="s">
         <v>1</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -2072,7 +1986,7 @@
       <c r="D42" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G42" s="14" t="s">
         <v>8</v>
       </c>
       <c r="H42" s="2" t="s">
@@ -2083,7 +1997,7 @@
       </c>
     </row>
     <row r="43" spans="2:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="2">
@@ -2092,7 +2006,7 @@
       <c r="D43" s="2">
         <v>5</v>
       </c>
-      <c r="G43" s="15" t="s">
+      <c r="G43" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H43" s="2">
@@ -2103,43 +2017,43 @@
       </c>
     </row>
     <row r="44" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="26" t="s">
-        <v>68</v>
+      <c r="B44" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G44" s="26" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="2:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B45" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>81</v>
+      <c r="B45" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G45" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="H45" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I45" s="29" t="s">
-        <v>73</v>
+      <c r="G45" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" s="22" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2148,9 +2062,9 @@
     <mergeCell ref="B32:Y32"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="G40:I40"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B9:R9"/>
     <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>